<commit_message>
fix table column formatting
</commit_message>
<xml_diff>
--- a/vedsite/generated/36a70659-5556-4ee6-ad66-f87e39e3d8be/211/table.xlsx
+++ b/vedsite/generated/36a70659-5556-4ee6-ad66-f87e39e3d8be/211/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD86333D-B3DC-4404-849E-6DACBE1173D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4035529D-4E8D-4202-853C-5FA88CC039F3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{EA7F0DAC-2E36-42A5-A800-D49062CC543D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Student</t>
   </si>
@@ -87,6 +87,9 @@
     <t>lolkek@edu.hse.ru</t>
   </si>
   <si>
+    <t>Памагите Пажождаааа</t>
+  </si>
+  <si>
     <t>pomogite@mail.ru</t>
   </si>
   <si>
@@ -94,9 +97,6 @@
   </si>
   <si>
     <t>nope@nope.nope</t>
-  </si>
-  <si>
-    <t>Памагите Пажождаааааааааааааааааааааааааааааааааааааааааааааааааааааааааааааа</t>
   </si>
 </sst>
 </file>
@@ -520,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A36B4A-B7AD-4C5B-9C24-4F7C0F99301A}">
-  <dimension ref="A1:AE7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AE7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +533,7 @@
     <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="1" t="s">
@@ -553,30 +553,8 @@
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
@@ -596,30 +574,8 @@
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -665,56 +621,8 @@
       <c r="O3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="4" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -762,59 +670,8 @@
         <f>SUM(M4:N4)</f>
         <v>1</v>
       </c>
-      <c r="P4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>1</v>
-      </c>
-      <c r="R4" s="4">
-        <v>1</v>
-      </c>
-      <c r="S4" s="4">
-        <v>1</v>
-      </c>
-      <c r="T4" s="4">
-        <v>1</v>
-      </c>
-      <c r="U4" s="4">
-        <v>1</v>
-      </c>
-      <c r="V4" s="4">
-        <v>1</v>
-      </c>
-      <c r="W4" s="4">
-        <v>1</v>
-      </c>
-      <c r="X4" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="4">
-        <f>SUM(P4:X4)</f>
-        <v>8</v>
-      </c>
-      <c r="Z4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="4">
-        <f>SUM(Z4:AA4)</f>
-        <v>1</v>
-      </c>
-      <c r="AC4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="4">
-        <f>SUM(AC4:AD4)</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -862,64 +719,13 @@
         <f t="shared" ref="O5:O7" si="1">SUM(M5:N5)</f>
         <v>2</v>
       </c>
-      <c r="P5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>0</v>
-      </c>
-      <c r="R5" s="4">
-        <v>0</v>
-      </c>
-      <c r="S5" s="4">
-        <v>0</v>
-      </c>
-      <c r="T5" s="4">
-        <v>0</v>
-      </c>
-      <c r="U5" s="4">
-        <v>0</v>
-      </c>
-      <c r="V5" s="4">
-        <v>0</v>
-      </c>
-      <c r="W5" s="4">
-        <v>0</v>
-      </c>
-      <c r="X5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="4">
-        <f t="shared" ref="Y5:Y6" si="2">SUM(P5:X5)</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="4">
-        <f t="shared" ref="AB5:AB7" si="3">SUM(Z5:AA5)</f>
-        <v>2</v>
-      </c>
-      <c r="AC5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="4">
-        <f t="shared" ref="AE5:AE7" si="4">SUM(AC5:AD5)</f>
-        <v>2</v>
-      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
@@ -962,64 +768,13 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P6" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>0</v>
-      </c>
-      <c r="R6" s="4">
-        <v>0</v>
-      </c>
-      <c r="S6" s="4">
-        <v>0</v>
-      </c>
-      <c r="T6" s="4">
-        <v>0</v>
-      </c>
-      <c r="U6" s="4">
-        <v>0</v>
-      </c>
-      <c r="V6" s="4">
-        <v>1</v>
-      </c>
-      <c r="W6" s="4">
-        <v>1</v>
-      </c>
-      <c r="X6" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="4">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="Z6" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="4">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AC6" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="4">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
@@ -1061,69 +816,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>0</v>
-      </c>
-      <c r="R7" s="4">
-        <v>0</v>
-      </c>
-      <c r="S7" s="4">
-        <v>0</v>
-      </c>
-      <c r="T7" s="4">
-        <v>0</v>
-      </c>
-      <c r="U7" s="4">
-        <v>0</v>
-      </c>
-      <c r="V7" s="4">
-        <v>0</v>
-      </c>
-      <c r="W7" s="4">
-        <v>0</v>
-      </c>
-      <c r="X7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="P2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AC2:AE2"/>
+  <mergeCells count="4">
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P1:Y1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{DF19BC3B-931D-4AC4-B135-53AA1B0860AB}"/>

</xml_diff>